<commit_message>
update by diabin lee
</commit_message>
<xml_diff>
--- a/bug-list.xlsx
+++ b/bug-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="288" windowWidth="14808" windowHeight="9300"/>
+    <workbookView xWindow="8100" yWindow="285" windowWidth="14805" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="bug-list" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>登陆页面的配置，点开后就无法关闭</t>
   </si>
@@ -368,6 +368,10 @@
   </si>
   <si>
     <t>v_1.2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功显示最新笔记信息</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -886,17 +890,17 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="64.109375" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="64.125" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -916,7 +920,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -938,7 +942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -949,7 +953,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -963,7 +967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -974,7 +978,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -988,7 +992,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1041,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1087,47 +1091,65 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
       <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1135,7 +1157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -1143,7 +1165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="46.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1160,7 +1182,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1168,7 +1190,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -1176,13 +1198,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
     </row>
   </sheetData>
@@ -1259,13 +1281,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="57.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.75" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1304,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -1293,7 +1315,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1304,7 +1326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1312,7 +1334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -1320,7 +1342,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1352,7 +1374,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>